<commit_message>
deleted old letsgodigital tess stuff added a fix for zero being recorded on a value change.
Signed-off-by: Hypothawits <tseccombe@gmail.com>
</commit_message>
<xml_diff>
--- a/Temperautre calibration.xlsx
+++ b/Temperautre calibration.xlsx
@@ -44,13 +44,13 @@
     <t>Kelvin</t>
   </si>
   <si>
-    <t>Ambient Themo (K)</t>
+    <t>Thermocouple (K)</t>
   </si>
   <si>
-    <t>Thermo (K)</t>
+    <t>Ambient Thermocouple (K)</t>
   </si>
   <si>
-    <t>Radar (K)</t>
+    <t>Infrared Thermometer  (K)</t>
   </si>
 </sst>
 </file>
@@ -69,15 +69,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -224,37 +230,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -281,11 +256,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -301,13 +394,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,60 +710,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5633-4C1D-B375-566458839267}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Difference</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0999999999999943</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.7000000000000028</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.7999999999999972</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5633-4C1D-B375-566458839267}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1550,7 +1642,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ambient Themo (K)</c:v>
+                  <c:v>Ambient Thermocouple (K)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1604,7 +1696,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Thermo (K)</c:v>
+                  <c:v>Thermocouple (K)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1654,11 +1746,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Radar (C)</c:v>
+                  <c:v>Infrared Thermometer  (K)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1700,60 +1792,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-DDB2-4616-90AB-86A33E7DFCDF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Difference</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$8:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.0999999999999659</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1000000000000227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.6999999999999886</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8000000000000114</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DDB2-4616-90AB-86A33E7DFCDF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1917,7 +1955,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-ZA"/>
-                  <a:t>Temperature (c)</a:t>
+                  <a:t>Temperature (K)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4857,14 +4895,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -4918,15 +4956,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5281,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,6 +5328,7 @@
     <col min="1" max="2" width="15.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5387,120 +5426,120 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="19">
         <f>B2+273</f>
         <v>289.10000000000002</v>
       </c>
-      <c r="C8" s="16">
-        <f t="shared" ref="C8:F8" si="2">C2+273</f>
+      <c r="C8" s="20">
+        <f t="shared" ref="C8:D8" si="2">C2+273</f>
         <v>288.39999999999998</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="21">
         <f t="shared" si="2"/>
         <v>287.3</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="20">
         <f>C8-D8</f>
         <v>1.0999999999999659</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="22">
         <f>E8/C8 *100</f>
         <v>0.38141470180303955</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
-        <f t="shared" ref="B9:F9" si="3">B3+273</f>
+      <c r="B9" s="23">
+        <f t="shared" ref="B9:D9" si="3">B3+273</f>
         <v>289.10000000000002</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="24">
         <f t="shared" si="3"/>
         <v>310.8</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="25">
         <f t="shared" si="3"/>
         <v>308.7</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="24">
         <f t="shared" ref="E9:E11" si="4">C9-D9</f>
         <v>2.1000000000000227</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="26">
         <f t="shared" ref="F9:F11" si="5">E9/C9 *100</f>
         <v>0.67567567567568299</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
-        <f t="shared" ref="B10:F10" si="6">B4+273</f>
+      <c r="B10" s="27">
+        <f t="shared" ref="B10:D10" si="6">B4+273</f>
         <v>289.10000000000002</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="28">
         <f t="shared" si="6"/>
         <v>327</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="29">
         <f t="shared" si="6"/>
         <v>320.3</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="28">
         <f t="shared" si="4"/>
         <v>6.6999999999999886</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="30">
         <f t="shared" si="5"/>
         <v>2.048929663608559</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
-        <f t="shared" ref="B11:F11" si="7">B5+273</f>
+      <c r="B11" s="31">
+        <f t="shared" ref="B11:D11" si="7">B5+273</f>
         <v>289.10000000000002</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="32">
         <f t="shared" si="7"/>
         <v>333</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="33">
         <f t="shared" si="7"/>
         <v>328.2</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="32">
         <f t="shared" si="4"/>
         <v>4.8000000000000114</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="34">
         <f t="shared" si="5"/>
         <v>1.4414414414414449</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>